<commit_message>
dotnet 10 Added examples
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Redbf2b18be714e55"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R261715061ae249cf"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -96,7 +96,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45949.85773707176</x:v>
+        <x:v>45976.82439765046</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -104,7 +104,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45949.85773707176</x:v>
+        <x:v>45976.82439765046</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
freeze frames and row height
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R261715061ae249cf"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R81454190e3b548f4"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -96,7 +96,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45976.82439765046</x:v>
+        <x:v>45976.88578993056</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -104,7 +104,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45976.82439765046</x:v>
+        <x:v>45976.88578993056</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
added features (text alignments and hyperlinks)
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R81454190e3b548f4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rabcd06d0903d4b4b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -96,7 +96,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45976.88578993056</x:v>
+        <x:v>45976.89761574074</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -104,7 +104,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45976.88578993056</x:v>
+        <x:v>45976.89761574074</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
added feature: cell merging
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R71f44017e2c04684"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rb199bccfe6644efc"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -96,7 +96,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45977.46785375</x:v>
+        <x:v>45977.48433409722</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -104,7 +104,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45977.46785376158</x:v>
+        <x:v>45977.48433409722</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Data validation and Named ranges
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rb199bccfe6644efc"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R9ff8a91f5d34402e"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -96,7 +96,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45977.48433409722</x:v>
+        <x:v>45977.496436203706</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -104,7 +104,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45977.48433409722</x:v>
+        <x:v>45977.496436203706</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
chart step 3 (bar chart)
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rec1ac481d42944b1"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R59698a9975fb4fa4"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -96,7 +96,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45977.60673078704</x:v>
+        <x:v>45977.65872157407</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -104,7 +104,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45977.60673078704</x:v>
+        <x:v>45977.65872158565</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
chart step 5 (additional charts)
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R59698a9975fb4fa4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R61b65a74b2e14c24"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -96,7 +96,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45977.65872157407</x:v>
+        <x:v>45977.67140265046</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -104,7 +104,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45977.65872158565</x:v>
+        <x:v>45977.67140265046</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added more formatting options to charts.
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R09943f3f84944179"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R4e171ef168ea43eb"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45979.410144409725</x:v>
+        <x:v>45979.97417868055</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45979.410144409725</x:v>
+        <x:v>45979.97417868055</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added helper for json file import.
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R4e171ef168ea43eb"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R0513bf8e98b74b1c"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45979.97417868055</x:v>
+        <x:v>45980.05897637732</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45979.97417868055</x:v>
+        <x:v>45980.05897637732</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
additional support for json import.
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R0513bf8e98b74b1c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R905f8bf6025a4f20"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45980.05897637732</x:v>
+        <x:v>45980.065381203705</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45980.05897637732</x:v>
+        <x:v>45980.065381203705</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added features to json-import.
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Ra234fabda047441d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R29d234cd44e2408b"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45980.239889375</x:v>
+        <x:v>45980.2592422338</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45980.239889375</x:v>
+        <x:v>45980.2592422338</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added colors. Reformat code, fixed styling, fixed typo in API
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R91c8e1a63c3249f5"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rc6ee9a37c3014e3e"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45981.1278283912</x:v>
+        <x:v>45981.228250486114</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45981.1278283912</x:v>
+        <x:v>45981.228250486114</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Target dotnet9 for backward compability
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rfd17b6dfda2d4354"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R3dda2d267f93404a"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>45993.425738715276</x:v>
+        <x:v>46003.08408594907</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>45993.425738715276</x:v>
+        <x:v>46003.08408594907</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add support for custom series names in charts
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R3dda2d267f93404a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R91ae84a904ba443e"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>46003.08408594907</x:v>
+        <x:v>46026.21636413194</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>46003.08408594907</x:v>
+        <x:v>46026.21636413194</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add example for multi-table multi-chart dashboard creation
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R91ae84a904ba443e"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R9ebba8f69e2c4626"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>46026.21636413194</x:v>
+        <x:v>46026.25985699074</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>46026.21636413194</x:v>
+        <x:v>46026.25985699074</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Hiding rows and columns
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/02_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rc2da0cb549214d13"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R3b79528e709342dc"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>46034.32543563657</x:v>
+        <x:v>46036.30166094907</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>46034.32543563657</x:v>
+        <x:v>46036.30166094907</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>